<commit_message>
fix invalid report file when convert to list
</commit_message>
<xml_diff>
--- a/FinancialPlanningBE/FinancialPlanning.Service/Template/Monthly Expense Report_Template.xlsx
+++ b/FinancialPlanningBE/FinancialPlanning.Service/Template/Monthly Expense Report_Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25906"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thuth3\Documents\FA SRS\Financial plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\FinancialPlanning\financial-planning\FinancialPlanningBE\FinancialPlanning.Service\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_E16202547D798ECB2E7A01A06068D778B72E0A27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8240"/>
   </bookViews>
   <sheets>
     <sheet name="Expense" sheetId="2" r:id="rId1"/>
@@ -163,12 +162,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.000\ [$₫-42A];\-#,##0.000\ [$₫-42A]"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -305,10 +304,29 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="Tiền tệ" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -585,31 +603,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" customWidth="1"/>
+    <col min="9" max="9" width="21.81640625" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" customWidth="1"/>
+    <col min="11" max="11" width="23.54296875" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -638,8 +656,8 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:12" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -676,141 +694,99 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="16"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="13">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0</v>
-      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="13"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="6"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="17"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="13">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0</v>
-      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="13"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="16"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="13">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="13">
-        <v>0</v>
-      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="13"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="6"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="17"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="13">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0</v>
-      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="13"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="16"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="13">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0</v>
-      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="13"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="18"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="13">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="13">
-        <v>0</v>
-      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="13"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
       <c r="K8" s="6"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="19"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="13">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0</v>
-      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="3"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -818,28 +794,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>List!$B$3:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>C3:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>List!$E$3:$E$6</xm:f>
           </x14:formula1>
           <xm:sqref>E3:E9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>List!$B$13:$B$17</xm:f>
           </x14:formula1>
           <xm:sqref>J3:J6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>List!$E$13:$E$17</xm:f>
           </x14:formula1>
@@ -852,23 +829,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="4.7265625" customWidth="1"/>
+    <col min="5" max="5" width="32.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
@@ -903,7 +880,7 @@
       <c r="AB1" s="8"/>
       <c r="AC1" s="8"/>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
@@ -942,7 +919,7 @@
       <c r="AB2" s="8"/>
       <c r="AC2" s="8"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -977,7 +954,7 @@
       <c r="AB3" s="8"/>
       <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>23</v>
@@ -1012,7 +989,7 @@
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>25</v>
@@ -1047,7 +1024,7 @@
       <c r="AB5" s="9"/>
       <c r="AC5" s="9"/>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>27</v>
@@ -1082,7 +1059,7 @@
       <c r="AB6" s="9"/>
       <c r="AC6" s="9"/>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>29</v>
@@ -1115,7 +1092,7 @@
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>30</v>
@@ -1148,7 +1125,7 @@
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>31</v>
@@ -1181,7 +1158,7 @@
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1212,7 +1189,7 @@
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>32</v>
       </c>
@@ -1247,7 +1224,7 @@
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
@@ -1286,7 +1263,7 @@
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>34</v>
@@ -1321,7 +1298,7 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>36</v>
@@ -1353,7 +1330,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>38</v>
@@ -1385,7 +1362,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>40</v>
@@ -1417,7 +1394,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
@@ -1449,7 +1426,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1477,7 +1454,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1505,7 +1482,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>

</xml_diff>